<commit_message>
update unit tests change to JenkinsModelAbstractItem for job base class
</commit_message>
<xml_diff>
--- a/Tools/Schema/APIs.xlsx
+++ b/Tools/Schema/APIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\JenkinsWebApi.xml\Tools\Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51723206-4319-427A-9B9C-A7A322E66042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2B3884-02D9-475D-8860-3C35D7C778C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="36" windowWidth="12264" windowHeight="8592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -297,7 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -306,6 +312,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
@@ -592,7 +599,7 @@
   <dimension ref="A2:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +658,7 @@
       <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -793,7 +800,7 @@
       <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -873,7 +880,7 @@
       <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="6" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>